<commit_message>
Updated Email body and Adjustments workflow
</commit_message>
<xml_diff>
--- a/Data/Input/FundsDistributions_TestCaseV4.0.xlsx
+++ b/Data/Input/FundsDistributions_TestCaseV4.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmahe\Documents\UiPath\FederalBotFactory\FundsDistribution\FundDistributions\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEAEC6A-9E8D-4A03-90C6-0267383F1BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C33B83-4DEB-45EA-B6F5-2383ED2D80EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{688C6AAD-5601-4545-9C7C-9E8F4B197C36}"/>
   </bookViews>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1A48C0-806C-4604-9A42-1CA060CE3249}">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,13 +828,13 @@
         <v>56</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X2" s="3">
         <v>1</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA2" s="3"/>
     </row>
@@ -906,13 +906,13 @@
         <v>56</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X3" s="3">
         <v>1</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA3" s="3"/>
     </row>
@@ -984,13 +984,13 @@
         <v>46</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA4" s="3"/>
     </row>
@@ -1062,13 +1062,13 @@
         <v>46</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AA5" s="3"/>
     </row>
@@ -1140,13 +1140,13 @@
         <v>51</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X6" s="3">
         <v>1</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:27" customFormat="1" x14ac:dyDescent="0.35">
@@ -1217,13 +1217,13 @@
         <v>51</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X7" s="3">
         <v>1</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
@@ -1294,13 +1294,13 @@
         <v>38</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
@@ -1371,13 +1371,13 @@
         <v>38</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="X9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">

</xml_diff>